<commit_message>
feat: Added ship api call
</commit_message>
<xml_diff>
--- a/neo4j/import/data.xlsx
+++ b/neo4j/import/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\Stellarium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Projects\Stellarium\neo4j\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247AFB6B-401D-49D7-82CE-258FA24BD6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B0B2E2-8A8A-4AD2-BDF6-F1CBB918DE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="players" sheetId="1" r:id="rId1"/>
@@ -1410,7 +1410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -2852,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,13 +2900,13 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2920,13 +2920,13 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2940,13 +2940,13 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2960,13 +2960,13 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2980,13 +2980,13 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3000,13 +3000,13 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3020,13 +3020,13 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3040,13 +3040,13 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3060,13 +3060,13 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3080,13 +3080,13 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3100,13 +3100,13 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3120,13 +3120,13 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -3140,13 +3140,13 @@
         <v>1</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E14">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3160,13 +3160,13 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E15">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -3180,13 +3180,13 @@
         <v>1</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3200,13 +3200,13 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3220,13 +3220,13 @@
         <v>1</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E18">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -3240,13 +3240,13 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3260,13 +3260,13 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E20">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3280,13 +3280,13 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3300,13 +3300,13 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E22">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3320,13 +3320,13 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -3340,13 +3340,13 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -3360,13 +3360,13 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E25">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F25">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -3380,13 +3380,13 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3400,13 +3400,13 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F27">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -3420,13 +3420,13 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E28">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F28">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -3440,13 +3440,13 @@
         <v>1</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -3460,13 +3460,13 @@
         <v>1</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3480,13 +3480,13 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F31">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>